<commit_message>
Header Section for Reports
</commit_message>
<xml_diff>
--- a/admin/NFA_ACTIVE_NO_ENROLLMENTS_REPORT.xlsx
+++ b/admin/NFA_ACTIVE_NO_ENROLLMENTS_REPORT.xlsx
@@ -23,7 +23,7 @@
     <t>Amto.Robert (Arthur Murray Thousand Oaks)</t>
   </si>
   <si>
-    <t>(01/01/2025 - 10/10/2025)</t>
+    <t>(10/12/2025 - 10/23/2025)</t>
   </si>
   <si>
     <t>Service Provider</t>
@@ -44,10 +44,10 @@
     <t>Coach Coach</t>
   </si>
   <si>
-    <t>Edwin Cabrera</t>
-  </si>
-  <si>
     <t>Nicholas Kavoklis</t>
+  </si>
+  <si>
+    <t>Roumyadeb Karmakar</t>
   </si>
   <si>
     <t>Total</t>
@@ -484,13 +484,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="5">
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D5" s="5">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="E5"/>
     </row>
@@ -499,13 +499,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="5">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C6" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D6" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E6"/>
     </row>
@@ -514,13 +514,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="5">
-        <v>199</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5">
-        <v>177</v>
+        <v>0</v>
       </c>
       <c r="E7"/>
     </row>
@@ -529,10 +529,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="5">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="D8" s="5">
         <v>0</v>
@@ -544,13 +544,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="3">
-        <v>429</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="D9" s="3">
-        <v>295</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>